<commit_message>
Update Test Case Document
</commit_message>
<xml_diff>
--- a/Test Case Document dan Hasil Manual Testing/Test Case Document Final Project (Itera-QA).xlsx
+++ b/Test Case Document dan Hasil Manual Testing/Test Case Document Final Project (Itera-QA).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="220">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -734,14 +734,14 @@
     </r>
   </si>
   <si>
-    <t>Create New Costumer Details</t>
+    <t>Create New Customer Details</t>
   </si>
   <si>
     <t>IT-15</t>
   </si>
   <si>
     <t>Verify 
-Create New Successfully</t>
+Create New Customer Successfully</t>
   </si>
   <si>
     <t>Fill in All Fields</t>
@@ -766,10 +766,10 @@
 </t>
   </si>
   <si>
-    <t>Success Create New Costumer Details</t>
-  </si>
-  <si>
-    <t>Success Create New Costumer Details and
+    <t>Success Create New Customer Details</t>
+  </si>
+  <si>
+    <t>Success Create New Customer Details and
  Redirect to Dashboard</t>
   </si>
   <si>
@@ -799,7 +799,7 @@
     <t>Fill All The Fields with The Same Data</t>
   </si>
   <si>
-    <t>Failed Create New Costumer Details</t>
+    <t>Failed Create New Customer Details</t>
   </si>
   <si>
     <t>New data is created and
@@ -975,7 +975,7 @@
     <t>Verify Search Successfully</t>
   </si>
   <si>
-    <t>Search Name or Email Costumer</t>
+    <t>Search by Name Customer</t>
   </si>
   <si>
     <t>1. Input Name or Email
@@ -999,7 +999,7 @@
     <t>Verify Search Failed</t>
   </si>
   <si>
-    <t>Search Uncreated Name or Email Costumer</t>
+    <t>Search Uncreated Name Customer</t>
   </si>
   <si>
     <t>Ga Ada</t>
@@ -1038,7 +1038,7 @@
     <t>Verify Edit Successfully</t>
   </si>
   <si>
-    <t>Edit Name Costumer</t>
+    <t>Edit Name Customer</t>
   </si>
   <si>
     <t>1. Click Edit button
@@ -1061,7 +1061,7 @@
     <t>IT-30</t>
   </si>
   <si>
-    <t>Edit Email Costumer</t>
+    <t>Edit Email Customer</t>
   </si>
   <si>
     <t>1. Click Edit Button
@@ -1091,7 +1091,7 @@
     <t>Verify Edit Failed</t>
   </si>
   <si>
-    <t>Blank Name Costumer Field</t>
+    <t>Blank Name Customer Field</t>
   </si>
   <si>
     <t>1. Click Edit Button
@@ -1111,7 +1111,7 @@
     <t>IT-33</t>
   </si>
   <si>
-    <t>Blank Email Costumer Field</t>
+    <t>Blank Email Customer Field</t>
   </si>
   <si>
     <t>1. Click Edit Button
@@ -1152,6 +1152,9 @@
     <t>Click Details Button</t>
   </si>
   <si>
+    <t>Name: Sanber</t>
+  </si>
+  <si>
     <t>Success Show Details Customer</t>
   </si>
   <si>
@@ -1206,8 +1209,11 @@
     <t>Delete Data Customer</t>
   </si>
   <si>
-    <t>1. Click Delete Button
-2. Click Detete Button</t>
+    <t>1. On page List Customer, click Delete Button
+2. Click Delete Button</t>
+  </si>
+  <si>
+    <t>Deleted customer: John</t>
   </si>
   <si>
     <t>Data deleted successfully</t>
@@ -1640,7 +1646,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -2972,18 +2981,20 @@
       <c r="E46" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="F46" s="22"/>
+      <c r="F46" s="22" t="s">
+        <v>197</v>
+      </c>
       <c r="G46" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I46" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J46" s="24" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K46" s="16" t="s">
         <v>20</v>
@@ -2991,22 +3002,22 @@
     </row>
     <row r="47" ht="70.5" customHeight="1">
       <c r="A47" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>193</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>16</v>
@@ -3026,10 +3037,10 @@
     </row>
     <row r="48" ht="59.25" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>87</v>
@@ -3059,17 +3070,17 @@
     </row>
     <row r="49" ht="42.0" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
         <v>189</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="10" t="s">
@@ -3090,7 +3101,7 @@
     </row>
     <row r="50">
       <c r="A50" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -3105,32 +3116,34 @@
     </row>
     <row r="51" ht="40.5" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>146</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="F51" s="22"/>
+        <v>214</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>215</v>
+      </c>
       <c r="G51" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="I51" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J51" s="24" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="K51" s="16" t="s">
         <v>20</v>
@@ -3138,17 +3151,17 @@
     </row>
     <row r="52" ht="42.0" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
         <v>146</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="10" t="s">

</xml_diff>